<commit_message>
adding data visualization to the QAQC report
</commit_message>
<xml_diff>
--- a/documents/test_data/test_protocols/MarineGEO_Fish-Seines_Spreadsheet_v0.5.0_SERC2019.xlsx
+++ b/documents/test_data/test_protocols/MarineGEO_Fish-Seines_Spreadsheet_v0.5.0_SERC2019.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rob\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/SERC/MarineGEO/data_portal/documents/test_data/test_protocols/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DEA6F3-41C8-C14D-923E-E7159348EFC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21060" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_metadata" sheetId="1" r:id="rId1"/>
@@ -532,7 +533,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -1013,7 +1014,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D9033100-A170-CC46-BADE-67D4CD4E6F42}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9033100-A170-CC46-BADE-67D4CD4E6F42}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1150,6 +1151,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1185,6 +1203,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1360,28 +1395,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="39.950000000000003" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="40" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="47.7109375" customWidth="1"/>
-    <col min="2" max="2" width="100.7109375" customWidth="1"/>
+    <col min="1" max="1" width="47.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="161.1" customHeight="1">
+    <row r="1" spans="1:2" ht="161" customHeight="1">
       <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="2" spans="1:2" ht="40" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>44</v>
       </c>
@@ -1389,7 +1424,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="3" spans="1:2" ht="40" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
@@ -1397,7 +1432,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="4" spans="1:2" ht="40" customHeight="1">
       <c r="A4" s="4" t="s">
         <v>46</v>
       </c>
@@ -1405,7 +1440,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="5" spans="1:2" ht="40" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>47</v>
       </c>
@@ -1413,7 +1448,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="6" spans="1:2" ht="40" customHeight="1">
       <c r="A6" s="4" t="s">
         <v>81</v>
       </c>
@@ -1421,7 +1456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="7" spans="1:2" ht="40" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>82</v>
       </c>
@@ -1429,7 +1464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="8" spans="1:2" ht="40" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>83</v>
       </c>
@@ -1437,19 +1472,19 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="9" spans="1:2" ht="40" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B9" s="12"/>
     </row>
-    <row r="10" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="10" spans="1:2" ht="40" customHeight="1">
       <c r="A10" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="12"/>
     </row>
-    <row r="11" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="11" spans="1:2" ht="40" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>50</v>
       </c>
@@ -1457,7 +1492,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="39.950000000000003" customHeight="1">
+    <row r="12" spans="1:2" ht="40" customHeight="1">
       <c r="A12" s="30" t="s">
         <v>51</v>
       </c>
@@ -1502,18 +1537,18 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="9">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of person to be contacted" sqref="A3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of data entry person(s)" sqref="A5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Note the version of the MarineGEO protocol referenced to collect these data" sqref="A10"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data of final data entry" sqref="A6:A8"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please note any special cirucumstances, unusual findings, data abnormalities, etc…that might impact the interpretation of these data" sqref="A9"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Overwrite the  square bracket contents to genereate a unique title for this datasheet" sqref="A2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="E-mail of the contact person" sqref="A4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The version number of this workbook" sqref="A11"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seriously, feel free to contact us!" sqref="A12"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name of person to be contacted" sqref="A3" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of data entry person(s)" sqref="A5" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Note the version of the MarineGEO protocol referenced to collect these data" sqref="A10" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data of final data entry" sqref="A6:A8" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please note any special cirucumstances, unusual findings, data abnormalities, etc…that might impact the interpretation of these data" sqref="A9" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Overwrite the  square bracket contents to genereate a unique title for this datasheet" sqref="A2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="E-mail of the contact person" sqref="A4" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The version number of this workbook" sqref="A11" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Seriously, feel free to contact us!" sqref="A12" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -1521,34 +1556,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
     <col min="6" max="6" width="22" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.1640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="1" customWidth="1"/>
-    <col min="12" max="14" width="19.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="21.42578125" style="42" customWidth="1"/>
-    <col min="16" max="16" width="21.42578125" customWidth="1"/>
-    <col min="17" max="17" width="27.140625" customWidth="1"/>
+    <col min="12" max="14" width="19.1640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5" style="42" customWidth="1"/>
+    <col min="16" max="16" width="21.5" customWidth="1"/>
+    <col min="17" max="17" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="35" customFormat="1" ht="30" customHeight="1">
@@ -1604,7 +1639,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="60">
+    <row r="2" spans="1:17" ht="48">
       <c r="A2" s="15">
         <v>43640</v>
       </c>
@@ -1657,7 +1692,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="45">
+    <row r="3" spans="1:17" ht="48">
       <c r="A3" s="15">
         <v>43640</v>
       </c>
@@ -1698,7 +1733,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="165">
+    <row r="4" spans="1:17" ht="128">
       <c r="A4" s="15">
         <v>44007</v>
       </c>
@@ -2029,49 +2064,49 @@
     </row>
   </sheetData>
   <dataValidations count="15">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field (YYYY-MM-DD)" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was processed in the lab (YYYY-MM-DD)" sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="F1 H1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Longitude in decimal degrees to five decimal places" sqref="G1 I1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Site depth in meters. _x000a__x000a_For sites spanning a depth range, please provide a single, average depth." sqref="J1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The mesh size on the beach seine, in millimeters" sqref="K1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The width of the beach seine, in meters" sqref="L1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The height of the beach seine, in meters" sqref="M1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The distance towed along the transect, in meters (may or may not be 50 m)" sqref="N1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes about the sample metadata" sqref="Q1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of data collector(s)" sqref="O1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Full name of the data entry person" sqref="P1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field (YYYY-MM-DD)" sqref="A1" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was processed in the lab (YYYY-MM-DD)" sqref="E1" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="F1 H1" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Longitude in decimal degrees to five decimal places" sqref="G1 I1" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Site depth in meters. _x000a__x000a_For sites spanning a depth range, please provide a single, average depth." sqref="J1" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The mesh size on the beach seine, in millimeters" sqref="K1" xr:uid="{00000000-0002-0000-0100-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The width of the beach seine, in meters" sqref="L1" xr:uid="{00000000-0002-0000-0100-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The height of the beach seine, in meters" sqref="M1" xr:uid="{00000000-0002-0000-0100-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The distance towed along the transect, in meters (may or may not be 50 m)" sqref="N1" xr:uid="{00000000-0002-0000-0100-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes about the sample metadata" sqref="Q1" xr:uid="{00000000-0002-0000-0100-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Name(s) of data collector(s)" sqref="O1" xr:uid="{00000000-0002-0000-0100-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Full name of the data entry person" sqref="P1" xr:uid="{00000000-0002-0000-0100-00000E000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="6" width="20.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="6" width="20.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="35" customFormat="1" ht="30">
+    <row r="1" spans="1:8" s="35" customFormat="1" ht="16">
       <c r="A1" s="33" t="s">
         <v>63</v>
       </c>
@@ -2864,21 +2899,21 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Abundance of each fish taxon. _x000d__x000a__x000d__x000a_For taxa with abundance &gt;1, record a value of 1 for all but the final entry. For the final entry, enter a Value = Total Abundance - Sum of 1's from above." sqref="G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field (YYYY-MM-DD)" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes regarding observations, context, or concerns about the data" sqref="H1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Scientific name using standard scientific nomenclature. If the species cannot be identified to species, report genus or higher." sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes regarding observations, context, or concerns about the data." sqref="F1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Abundance of each fish taxon. _x000d__x000a__x000d__x000a_For taxa with abundance &gt;1, record a value of 1 for all but the final entry. For the final entry, enter a Value = Total Abundance - Sum of 1's from above." sqref="G1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field (YYYY-MM-DD)" sqref="A1" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1" xr:uid="{00000000-0002-0000-0200-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1" xr:uid="{00000000-0002-0000-0200-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes regarding observations, context, or concerns about the data" sqref="H1" xr:uid="{00000000-0002-0000-0200-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Scientific name using standard scientific nomenclature. If the species cannot be identified to species, report genus or higher." sqref="E1" xr:uid="{00000000-0002-0000-0200-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes regarding observations, context, or concerns about the data." sqref="F1" xr:uid="{00000000-0002-0000-0200-000007000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -2888,16 +2923,16 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="7" width="20.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="21.5" customWidth="1"/>
+    <col min="5" max="7" width="20.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="35" customFormat="1" ht="30">
+    <row r="1" spans="1:8" s="35" customFormat="1" ht="16">
       <c r="A1" s="33" t="s">
         <v>63</v>
       </c>
@@ -6085,21 +6120,21 @@
     </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes regarding observations, context, or concerns about the data." sqref="F1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Scientific name using standard scientific nomenclature. If the species cannot be identified to species, report genus or higher." sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes regarding observations, context, or concerns about the data" sqref="H1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field (YYYY-MM-DD)" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Length, in millimeters, of the first 20 individuals per taxon._x000d__x000a__x000d__x000a_Each cell should contain only one length measurement." sqref="G1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes regarding observations, context, or concerns about the data." sqref="F1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Scientific name using standard scientific nomenclature. If the species cannot be identified to species, report genus or higher." sqref="E1" xr:uid="{00000000-0002-0000-0300-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Any additional notes regarding observations, context, or concerns about the data" sqref="H1" xr:uid="{00000000-0002-0000-0300-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter your 6 character code (XXX-YYY). _x000a__x000a_Codes can be found in the standards section of the MarineGEO protocol website @ https://marinegeo.github.io/standards/" sqref="B1" xr:uid="{00000000-0002-0000-0300-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the specific location where the sample was collected; e.g., Curlew Cay" sqref="C1" xr:uid="{00000000-0002-0000-0300-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The date the sample was collected in the field (YYYY-MM-DD)" sqref="A1" xr:uid="{00000000-0002-0000-0300-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The transect at the location the sample came from: 1, 2, or 3" sqref="D1" xr:uid="{00000000-0002-0000-0300-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Length, in millimeters, of the first 20 individuals per taxon._x000d__x000a__x000d__x000a_Each cell should contain only one length measurement." sqref="G1" xr:uid="{00000000-0002-0000-0300-000007000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
@@ -6110,17 +6145,17 @@
       <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="50.1" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="50" customHeight="1"/>
   <cols>
-    <col min="1" max="3" width="40.7109375" style="27" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="27" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" style="27" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="27" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="26" customWidth="1"/>
-    <col min="8" max="16384" width="8.85546875" style="26"/>
+    <col min="1" max="3" width="40.6640625" style="27" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" style="27" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="27" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="26" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="28" customFormat="1" ht="15.75">
+    <row r="1" spans="1:6" s="28" customFormat="1" ht="17">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -6140,7 +6175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="21" customFormat="1" ht="56.1" customHeight="1">
+    <row r="2" spans="1:6" s="21" customFormat="1" ht="56" customHeight="1">
       <c r="A2" s="17" t="s">
         <v>58</v>
       </c>
@@ -6152,7 +6187,7 @@
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="3" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>58</v>
       </c>
@@ -6168,7 +6203,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="4" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>58</v>
       </c>
@@ -6184,7 +6219,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="5" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>58</v>
       </c>
@@ -6200,7 +6235,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="6" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>58</v>
       </c>
@@ -6234,7 +6269,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="8" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>58</v>
       </c>
@@ -6252,7 +6287,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="9" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>58</v>
       </c>
@@ -6270,7 +6305,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" s="21" customFormat="1" ht="56.1" customHeight="1">
+    <row r="10" spans="1:6" s="21" customFormat="1" ht="56" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>58</v>
       </c>
@@ -6322,7 +6357,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="13" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A13" s="6" t="s">
         <v>58</v>
       </c>
@@ -6338,7 +6373,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="14" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A14" s="17" t="s">
         <v>60</v>
       </c>
@@ -6368,7 +6403,7 @@
       </c>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="16" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A16" s="7" t="s">
         <v>60</v>
       </c>
@@ -6384,7 +6419,7 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="17" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A17" s="7" t="s">
         <v>60</v>
       </c>
@@ -6434,7 +6469,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="20" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A20" s="7" t="s">
         <v>60</v>
       </c>
@@ -6450,7 +6485,7 @@
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="21" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>60</v>
       </c>
@@ -6468,7 +6503,7 @@
       </c>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="22" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A22" s="7" t="s">
         <v>60</v>
       </c>
@@ -6486,7 +6521,7 @@
       </c>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="23" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A23" s="7" t="s">
         <v>60</v>
       </c>
@@ -6504,7 +6539,7 @@
       </c>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="24" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -6522,7 +6557,7 @@
       </c>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="25" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A25" s="7" t="s">
         <v>60</v>
       </c>
@@ -6540,7 +6575,7 @@
       </c>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="26" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A26" s="7" t="s">
         <v>60</v>
       </c>
@@ -6558,7 +6593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="28" customFormat="1" ht="56.1" customHeight="1">
+    <row r="27" spans="1:6" s="28" customFormat="1" ht="56" customHeight="1">
       <c r="A27" s="7" t="s">
         <v>60</v>
       </c>
@@ -6576,7 +6611,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="21" customFormat="1" ht="56.1" customHeight="1">
+    <row r="28" spans="1:6" s="21" customFormat="1" ht="56" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>60</v>
       </c>
@@ -6594,7 +6629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="21" customFormat="1" ht="56.1" customHeight="1">
+    <row r="29" spans="1:6" s="21" customFormat="1" ht="56" customHeight="1">
       <c r="A29" s="7" t="s">
         <v>60</v>
       </c>
@@ -6612,7 +6647,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="28" customFormat="1" ht="31.5">
+    <row r="30" spans="1:6" s="28" customFormat="1" ht="34">
       <c r="A30" s="7" t="s">
         <v>60</v>
       </c>
@@ -6630,7 +6665,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="28" customFormat="1" ht="47.25">
+    <row r="31" spans="1:6" s="28" customFormat="1" ht="34">
       <c r="A31" s="7" t="s">
         <v>60</v>
       </c>
@@ -6646,7 +6681,7 @@
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:6" s="28" customFormat="1" ht="31.5">
+    <row r="32" spans="1:6" s="28" customFormat="1" ht="17">
       <c r="A32" s="17" t="s">
         <v>61</v>
       </c>
@@ -6710,7 +6745,7 @@
       </c>
       <c r="F35" s="29"/>
     </row>
-    <row r="36" spans="1:6" s="40" customFormat="1" ht="47.25">
+    <row r="36" spans="1:6" s="40" customFormat="1" ht="51">
       <c r="A36" s="14" t="s">
         <v>61</v>
       </c>
@@ -6726,7 +6761,7 @@
       <c r="E36" s="39"/>
       <c r="F36" s="39"/>
     </row>
-    <row r="37" spans="1:6" s="23" customFormat="1" ht="50.1" customHeight="1">
+    <row r="37" spans="1:6" s="23" customFormat="1" ht="50" customHeight="1">
       <c r="A37" s="14" t="s">
         <v>61</v>
       </c>
@@ -6788,7 +6823,7 @@
       <c r="E40" s="29"/>
       <c r="F40" s="29"/>
     </row>
-    <row r="41" spans="1:6" s="19" customFormat="1" ht="50.1" customHeight="1">
+    <row r="41" spans="1:6" s="19" customFormat="1" ht="50" customHeight="1">
       <c r="A41" s="14" t="s">
         <v>61</v>
       </c>
@@ -6804,7 +6839,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="19" customFormat="1" ht="50.1" customHeight="1">
+    <row r="42" spans="1:6" s="19" customFormat="1" ht="50" customHeight="1">
       <c r="A42" s="14" t="s">
         <v>61</v>
       </c>
@@ -6820,7 +6855,7 @@
       <c r="E42" s="29"/>
       <c r="F42" s="32"/>
     </row>
-    <row r="43" spans="1:6" ht="50.1" customHeight="1">
+    <row r="43" spans="1:6" ht="50" customHeight="1">
       <c r="A43" s="17" t="s">
         <v>53</v>
       </c>
@@ -6832,7 +6867,7 @@
       <c r="E43" s="18"/>
       <c r="F43" s="17"/>
     </row>
-    <row r="44" spans="1:6" ht="50.1" customHeight="1">
+    <row r="44" spans="1:6" ht="50" customHeight="1">
       <c r="A44" s="7" t="s">
         <v>53</v>
       </c>
@@ -6848,7 +6883,7 @@
       <c r="E44" s="11"/>
       <c r="F44" s="7"/>
     </row>
-    <row r="45" spans="1:6" ht="50.1" customHeight="1">
+    <row r="45" spans="1:6" ht="50" customHeight="1">
       <c r="A45" s="7" t="s">
         <v>53</v>
       </c>
@@ -6864,7 +6899,7 @@
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
     </row>
-    <row r="46" spans="1:6" ht="50.1" customHeight="1">
+    <row r="46" spans="1:6" ht="50" customHeight="1">
       <c r="A46" s="7" t="s">
         <v>53</v>
       </c>
@@ -6880,7 +6915,7 @@
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
     </row>
-    <row r="47" spans="1:6" ht="50.1" customHeight="1">
+    <row r="47" spans="1:6" ht="50" customHeight="1">
       <c r="A47" s="7" t="s">
         <v>53</v>
       </c>
@@ -6896,7 +6931,7 @@
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
     </row>
-    <row r="48" spans="1:6" ht="50.1" customHeight="1">
+    <row r="48" spans="1:6" ht="50" customHeight="1">
       <c r="A48" s="7" t="s">
         <v>53</v>
       </c>
@@ -6912,7 +6947,7 @@
       <c r="E48" s="11"/>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="1:6" ht="50.1" customHeight="1">
+    <row r="49" spans="1:6" ht="50" customHeight="1">
       <c r="A49" s="7" t="s">
         <v>53</v>
       </c>
@@ -6950,15 +6985,15 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="9">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Longitude in decimal degrees to five decimal places" sqref="B23 B25 B27:B30"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="B24 B22"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="B40"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The units the field should contain" sqref="F1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The format the field should follow" sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The type of entry that should occupy the field (e.g., text, decimal, integer, date, etc…)" sqref="D1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The field definition" sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the field being defined" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The sheet in which the field occurs" sqref="A1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Longitude in decimal degrees to five decimal places" sqref="B23 B25 B27:B30" xr:uid="{00000000-0002-0000-0400-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="B24 B22" xr:uid="{00000000-0002-0000-0400-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A unique identifier used to identify a single taxon. Does not have to be a full scientific name, it can be a abbreviation or other, but in that case YOU MUST link that to scientific nomenclature in the 'TaxaList' sheet" sqref="B40" xr:uid="{00000000-0002-0000-0400-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The units the field should contain" sqref="F1" xr:uid="{00000000-0002-0000-0400-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The format the field should follow" sqref="E1" xr:uid="{00000000-0002-0000-0400-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The type of entry that should occupy the field (e.g., text, decimal, integer, date, etc…)" sqref="D1" xr:uid="{00000000-0002-0000-0400-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The field definition" sqref="C1" xr:uid="{00000000-0002-0000-0400-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The name of the field being defined" sqref="B1" xr:uid="{00000000-0002-0000-0400-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The sheet in which the field occurs" sqref="A1" xr:uid="{00000000-0002-0000-0400-000008000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>